<commit_message>
Diff and initial highlighting now work
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">Example Table1</t>
   </si>
   <si>
-    <t xml:space="preserve">The last row (which will be ignored) has some junk at the end.</t>
+    <t xml:space="preserve">This is a leading line, before the table</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
@@ -38,46 +38,70 @@
     <t xml:space="preserve">Fruit</t>
   </si>
   <si>
+    <t xml:space="preserve">Origin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Color</t>
   </si>
   <si>
     <t xml:space="preserve">apple</t>
   </si>
   <si>
+    <t xml:space="preserve">Maine</t>
+  </si>
+  <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
     <t xml:space="preserve">banana</t>
   </si>
   <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
     <t xml:space="preserve">yellow</t>
   </si>
   <si>
     <t xml:space="preserve">coconut</t>
   </si>
   <si>
+    <t xml:space="preserve">Hawaii</t>
+  </si>
+  <si>
     <t xml:space="preserve">brown</t>
   </si>
   <si>
     <t xml:space="preserve">dried mango</t>
   </si>
   <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
     <t xml:space="preserve">orange</t>
   </si>
   <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
     <t xml:space="preserve">Example Table2</t>
   </si>
   <si>
+    <t xml:space="preserve">Shape</t>
+  </si>
+  <si>
     <t xml:space="preserve">grapes</t>
   </si>
   <si>
+    <t xml:space="preserve">pebbles</t>
+  </si>
+  <si>
     <t xml:space="preserve">purple</t>
   </si>
   <si>
     <t xml:space="preserve">mango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flat</t>
   </si>
 </sst>
 </file>
@@ -204,10 +228,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -235,6 +259,9 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -244,10 +271,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -258,10 +288,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,10 +305,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,20 +322,21 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -317,17 +354,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,82 +374,66 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>44896</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>44915</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>44870</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>2</v>
-      </c>
       <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>44886</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>